<commit_message>
update planning and project structur
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\MAS-RAD\projet\AppBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241E2A7-F698-469A-B634-6560820DFC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF03D0-8109-429C-A220-16C6519774B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE222268-6C08-4172-89F8-531D515D3EF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE222268-6C08-4172-89F8-531D515D3EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$Q$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Mai</t>
   </si>
@@ -129,15 +132,6 @@
     <t>Mardi 17</t>
   </si>
   <si>
-    <t>Interface utilisateur</t>
-  </si>
-  <si>
-    <t>Interface utilisteur</t>
-  </si>
-  <si>
-    <t>Implémentation des fonctionalités</t>
-  </si>
-  <si>
     <t>Préparation de la présentation</t>
   </si>
   <si>
@@ -145,6 +139,18 @@
   </si>
   <si>
     <t>Présentation</t>
+  </si>
+  <si>
+    <t>Interface utilisateur (Application.class, WindowPrincipal.class, WindowMenu)</t>
+  </si>
+  <si>
+    <t>Interface utilisteur (WindowMenu.class, WindowTable.class, WindowButton)</t>
+  </si>
+  <si>
+    <t>Implémentation des fonctionalités(OpenAndSave.class)</t>
+  </si>
+  <si>
+    <t>Implémentation des fonctionalités (WindowPrincipal.class,  WindowTable.class)</t>
   </si>
 </sst>
 </file>
@@ -212,19 +218,184 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,22 +404,91 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,286 +805,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2796712C-6B51-4630-AD93-E919B1DF97A4}">
-  <dimension ref="A2:P19"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" customWidth="1"/>
-    <col min="2" max="8" width="10.6328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.6328125" style="2" customWidth="1"/>
-    <col min="10" max="16" width="10.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="8" width="12.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="1.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16" width="12.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C4" s="20"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="28"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P9" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="21"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="10"/>
+      <c r="P11" s="30"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="24"/>
+      <c r="C18" s="28"/>
+    </row>
+    <row r="19" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B17:P17"/>
+  <mergeCells count="9">
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B8:P8"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:P5"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update planning and readme
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\MAS-RAD\projet\AppBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF03D0-8109-429C-A220-16C6519774B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A59DE40-44F4-4599-BFCF-A557868A5C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE222268-6C08-4172-89F8-531D515D3EF9}"/>
   </bookViews>
@@ -141,16 +141,16 @@
     <t>Présentation</t>
   </si>
   <si>
-    <t>Interface utilisateur (Application.class, WindowPrincipal.class, WindowMenu)</t>
-  </si>
-  <si>
-    <t>Interface utilisteur (WindowMenu.class, WindowTable.class, WindowButton)</t>
-  </si>
-  <si>
-    <t>Implémentation des fonctionalités(OpenAndSave.class)</t>
-  </si>
-  <si>
-    <t>Implémentation des fonctionalités (WindowPrincipal.class,  WindowTable.class)</t>
+    <t>Implémentation des fonctionalités(OpenAndSave.java)</t>
+  </si>
+  <si>
+    <t>Interface utilisateur (Application.java, WindowPrincipal.java, WindowMenu)</t>
+  </si>
+  <si>
+    <t>Interface utilisteur (WindowMenu.java, WindowTable.java, WindowButton)</t>
+  </si>
+  <si>
+    <t>Implémentation des fonctionalités (WindowPrincipal.java,  WindowTable.java)</t>
   </si>
 </sst>
 </file>
@@ -413,82 +413,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2796712C-6B51-4630-AD93-E919B1DF97A4}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,71 +823,71 @@
     <row r="1" spans="1:16" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="15" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="17"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="C4" s="20"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -900,45 +900,45 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="21"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+        <v>35</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="23"/>
+      <c r="J5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="28"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="16"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -958,73 +958,73 @@
     </row>
     <row r="8" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1038,49 +1038,49 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="21"/>
+      <c r="P10" s="11"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="10" t="s">
+      <c r="J11" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="32"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="28"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="16"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="14" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1122,31 +1122,31 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1174,15 +1174,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="B8:P8"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:P5"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>